<commit_message>
adding inventory for ammonia
</commit_message>
<xml_diff>
--- a/electrolyzers_LCI.xlsx
+++ b/electrolyzers_LCI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsteinbach\PycharmProjects\HySPI app\HySPI_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2ECB631-F316-455A-B374-5B83CA7AFB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0E390C-47AB-4759-8B14-DC1FFFDF612E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1EA9BED0-42EC-4F80-9B46-2A73048EBAB6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="421">
   <si>
     <t>skip</t>
   </si>
@@ -1264,6 +1264,69 @@
   </si>
   <si>
     <t>used fuel cell balance of plant, 1MWe, AEC</t>
+  </si>
+  <si>
+    <t>ammonia production, steam reforming, liquid</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>market for chemical factory, organics</t>
+  </si>
+  <si>
+    <t>market group for municipal solid waste</t>
+  </si>
+  <si>
+    <t>market for solvent, organic</t>
+  </si>
+  <si>
+    <t>market for tap water</t>
+  </si>
+  <si>
+    <t>market for electricity, low voltage</t>
+  </si>
+  <si>
+    <t>market for natural gas, high pressure</t>
+  </si>
+  <si>
+    <t>chemical factory, organics</t>
+  </si>
+  <si>
+    <t>municipal solid waste</t>
+  </si>
+  <si>
+    <t>solvent, organic</t>
+  </si>
+  <si>
+    <t>tap water</t>
+  </si>
+  <si>
+    <t>natural gas, high pressure</t>
+  </si>
+  <si>
+    <t>air - urban air close to ground</t>
+  </si>
+  <si>
+    <t>water - surface water</t>
+  </si>
+  <si>
+    <t>natural resource - in water</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Nitrogen</t>
+  </si>
+  <si>
+    <t>Water, cooling, unspecified natural origin</t>
+  </si>
+  <si>
+    <t>ammonia, anhydrous, liquid</t>
+  </si>
+  <si>
+    <t>adapted from ecoinvent data</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1449,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1438,6 +1501,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE4D6"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1535,7 +1604,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1728,12 +1797,31 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="7" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1743,6 +1831,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2184,8 +2277,8 @@
       <c r="F12"/>
     </row>
     <row r="13" spans="1:7" ht="14.5">
-      <c r="B13" s="158"/>
-      <c r="C13" s="158"/>
+      <c r="B13" s="173"/>
+      <c r="C13" s="173"/>
       <c r="E13"/>
       <c r="F13"/>
     </row>
@@ -2555,10 +2648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E518564-62B5-463A-BC83-0EAFF50C141D}">
-  <dimension ref="A1:AO459"/>
+  <dimension ref="A1:AO489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD32"/>
+    <sheetView tabSelected="1" topLeftCell="A469" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B489" sqref="B489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
@@ -4177,8 +4270,8 @@
       <c r="S43" s="15"/>
       <c r="T43" s="15"/>
       <c r="Y43" s="15"/>
-      <c r="AK43" s="159"/>
-      <c r="AL43" s="159"/>
+      <c r="AK43" s="174"/>
+      <c r="AL43" s="174"/>
     </row>
     <row r="44" spans="1:38" s="51" customFormat="1">
       <c r="A44" s="105" t="s">
@@ -4216,8 +4309,8 @@
       <c r="S44" s="15"/>
       <c r="T44" s="15"/>
       <c r="Y44" s="15"/>
-      <c r="AK44" s="159"/>
-      <c r="AL44" s="159"/>
+      <c r="AK44" s="174"/>
+      <c r="AL44" s="174"/>
     </row>
     <row r="45" spans="1:38" s="51" customFormat="1">
       <c r="A45" s="105" t="s">
@@ -4255,8 +4348,8 @@
       <c r="S45" s="15"/>
       <c r="T45" s="15"/>
       <c r="Y45" s="15"/>
-      <c r="AK45" s="159"/>
-      <c r="AL45" s="159"/>
+      <c r="AK45" s="174"/>
+      <c r="AL45" s="174"/>
     </row>
     <row r="46" spans="1:38" s="51" customFormat="1">
       <c r="A46" s="105" t="s">
@@ -4294,8 +4387,8 @@
       <c r="S46" s="15"/>
       <c r="T46" s="15"/>
       <c r="Y46" s="15"/>
-      <c r="AK46" s="159"/>
-      <c r="AL46" s="159"/>
+      <c r="AK46" s="174"/>
+      <c r="AL46" s="174"/>
     </row>
     <row r="47" spans="1:38" s="51" customFormat="1">
       <c r="A47" s="105" t="s">
@@ -4333,8 +4426,8 @@
       <c r="S47" s="15"/>
       <c r="T47" s="15"/>
       <c r="Y47" s="15"/>
-      <c r="AK47" s="159"/>
-      <c r="AL47" s="159"/>
+      <c r="AK47" s="174"/>
+      <c r="AL47" s="174"/>
     </row>
     <row r="48" spans="1:38" s="51" customFormat="1">
       <c r="A48" s="105" t="s">
@@ -4372,8 +4465,8 @@
       <c r="S48" s="15"/>
       <c r="T48" s="15"/>
       <c r="Y48" s="15"/>
-      <c r="AK48" s="159"/>
-      <c r="AL48" s="159"/>
+      <c r="AK48" s="174"/>
+      <c r="AL48" s="174"/>
     </row>
     <row r="49" spans="1:38" s="51" customFormat="1">
       <c r="A49" s="105" t="s">
@@ -4411,8 +4504,8 @@
       <c r="S49" s="15"/>
       <c r="T49" s="15"/>
       <c r="Y49" s="15"/>
-      <c r="AK49" s="159"/>
-      <c r="AL49" s="159"/>
+      <c r="AK49" s="174"/>
+      <c r="AL49" s="174"/>
     </row>
     <row r="50" spans="1:38" s="51" customFormat="1">
       <c r="A50" s="105" t="s">
@@ -4450,8 +4543,8 @@
       <c r="S50" s="15"/>
       <c r="T50" s="15"/>
       <c r="Y50" s="15"/>
-      <c r="AK50" s="159"/>
-      <c r="AL50" s="159"/>
+      <c r="AK50" s="174"/>
+      <c r="AL50" s="174"/>
     </row>
     <row r="51" spans="1:38" s="51" customFormat="1">
       <c r="A51" s="105" t="s">
@@ -4489,8 +4582,8 @@
       <c r="S51" s="15"/>
       <c r="T51" s="15"/>
       <c r="Y51" s="15"/>
-      <c r="AK51" s="159"/>
-      <c r="AL51" s="159"/>
+      <c r="AK51" s="174"/>
+      <c r="AL51" s="174"/>
     </row>
     <row r="52" spans="1:38" s="51" customFormat="1">
       <c r="A52" s="103" t="s">
@@ -4528,8 +4621,8 @@
       <c r="S52" s="15"/>
       <c r="T52" s="15"/>
       <c r="Y52" s="15"/>
-      <c r="AK52" s="159"/>
-      <c r="AL52" s="159"/>
+      <c r="AK52" s="174"/>
+      <c r="AL52" s="174"/>
     </row>
     <row r="53" spans="1:38" s="51" customFormat="1">
       <c r="A53" s="102" t="s">
@@ -4567,8 +4660,8 @@
       <c r="S53" s="15"/>
       <c r="T53" s="15"/>
       <c r="Y53" s="15"/>
-      <c r="AK53" s="159"/>
-      <c r="AL53" s="159"/>
+      <c r="AK53" s="174"/>
+      <c r="AL53" s="174"/>
     </row>
     <row r="54" spans="1:38" s="51" customFormat="1">
       <c r="A54" s="105" t="s">
@@ -4606,8 +4699,8 @@
       <c r="S54" s="15"/>
       <c r="T54" s="15"/>
       <c r="Y54" s="15"/>
-      <c r="AK54" s="159"/>
-      <c r="AL54" s="159"/>
+      <c r="AK54" s="174"/>
+      <c r="AL54" s="174"/>
     </row>
     <row r="55" spans="1:38" s="51" customFormat="1">
       <c r="A55" s="103" t="s">
@@ -4645,8 +4738,8 @@
       <c r="S55" s="15"/>
       <c r="T55" s="15"/>
       <c r="Y55" s="15"/>
-      <c r="AK55" s="159"/>
-      <c r="AL55" s="159"/>
+      <c r="AK55" s="174"/>
+      <c r="AL55" s="174"/>
     </row>
     <row r="56" spans="1:38" s="51" customFormat="1">
       <c r="A56" s="102" t="s">
@@ -4684,8 +4777,8 @@
       <c r="S56" s="15"/>
       <c r="T56" s="15"/>
       <c r="Y56" s="15"/>
-      <c r="AK56" s="159"/>
-      <c r="AL56" s="159"/>
+      <c r="AK56" s="174"/>
+      <c r="AL56" s="174"/>
     </row>
     <row r="57" spans="1:38" s="51" customFormat="1">
       <c r="A57" s="105" t="s">
@@ -4723,8 +4816,8 @@
       <c r="S57" s="15"/>
       <c r="T57" s="15"/>
       <c r="Y57" s="15"/>
-      <c r="AK57" s="159"/>
-      <c r="AL57" s="159"/>
+      <c r="AK57" s="174"/>
+      <c r="AL57" s="174"/>
     </row>
     <row r="58" spans="1:38" s="51" customFormat="1">
       <c r="A58" s="103" t="s">
@@ -4762,8 +4855,8 @@
       <c r="S58" s="15"/>
       <c r="T58" s="15"/>
       <c r="Y58" s="15"/>
-      <c r="AK58" s="159"/>
-      <c r="AL58" s="159"/>
+      <c r="AK58" s="174"/>
+      <c r="AL58" s="174"/>
     </row>
     <row r="59" spans="1:38" s="51" customFormat="1">
       <c r="A59" s="102" t="s">
@@ -4801,8 +4894,8 @@
       <c r="S59" s="15"/>
       <c r="T59" s="15"/>
       <c r="Y59" s="15"/>
-      <c r="AK59" s="159"/>
-      <c r="AL59" s="159"/>
+      <c r="AK59" s="174"/>
+      <c r="AL59" s="174"/>
     </row>
     <row r="60" spans="1:38" s="51" customFormat="1">
       <c r="A60" s="105" t="s">
@@ -4840,8 +4933,8 @@
       <c r="S60" s="15"/>
       <c r="T60" s="15"/>
       <c r="Y60" s="15"/>
-      <c r="AK60" s="159"/>
-      <c r="AL60" s="159"/>
+      <c r="AK60" s="174"/>
+      <c r="AL60" s="174"/>
     </row>
     <row r="61" spans="1:38" s="51" customFormat="1" ht="17.5">
       <c r="A61" s="105" t="s">
@@ -4879,8 +4972,8 @@
       <c r="S61" s="15"/>
       <c r="T61" s="15"/>
       <c r="Y61" s="15"/>
-      <c r="AK61" s="159"/>
-      <c r="AL61" s="159"/>
+      <c r="AK61" s="174"/>
+      <c r="AL61" s="174"/>
     </row>
     <row r="62" spans="1:38" s="51" customFormat="1" ht="17.5">
       <c r="A62" s="103" t="s">
@@ -4918,8 +5011,8 @@
       <c r="S62" s="15"/>
       <c r="T62" s="15"/>
       <c r="Y62" s="15"/>
-      <c r="AK62" s="159"/>
-      <c r="AL62" s="159"/>
+      <c r="AK62" s="174"/>
+      <c r="AL62" s="174"/>
     </row>
     <row r="63" spans="1:38" s="51" customFormat="1">
       <c r="A63" s="102" t="s">
@@ -4957,8 +5050,8 @@
       <c r="S63" s="15"/>
       <c r="T63" s="15"/>
       <c r="Y63" s="15"/>
-      <c r="AK63" s="159"/>
-      <c r="AL63" s="159"/>
+      <c r="AK63" s="174"/>
+      <c r="AL63" s="174"/>
     </row>
     <row r="64" spans="1:38" s="51" customFormat="1">
       <c r="A64" s="105" t="s">
@@ -4996,8 +5089,8 @@
       <c r="S64" s="15"/>
       <c r="T64" s="15"/>
       <c r="Y64" s="15"/>
-      <c r="AK64" s="159"/>
-      <c r="AL64" s="159"/>
+      <c r="AK64" s="174"/>
+      <c r="AL64" s="174"/>
     </row>
     <row r="65" spans="1:38" s="51" customFormat="1">
       <c r="A65" s="103" t="s">
@@ -5035,8 +5128,8 @@
       <c r="S65" s="15"/>
       <c r="T65" s="15"/>
       <c r="Y65" s="15"/>
-      <c r="AK65" s="159"/>
-      <c r="AL65" s="159"/>
+      <c r="AK65" s="174"/>
+      <c r="AL65" s="174"/>
     </row>
     <row r="66" spans="1:38" s="51" customFormat="1">
       <c r="A66" s="102" t="s">
@@ -5074,8 +5167,8 @@
       <c r="S66" s="15"/>
       <c r="T66" s="15"/>
       <c r="Y66" s="15"/>
-      <c r="AK66" s="159"/>
-      <c r="AL66" s="159"/>
+      <c r="AK66" s="174"/>
+      <c r="AL66" s="174"/>
     </row>
     <row r="67" spans="1:38" s="51" customFormat="1">
       <c r="A67" s="105" t="s">
@@ -5113,8 +5206,8 @@
       <c r="S67" s="15"/>
       <c r="T67" s="15"/>
       <c r="Y67" s="15"/>
-      <c r="AK67" s="159"/>
-      <c r="AL67" s="159"/>
+      <c r="AK67" s="174"/>
+      <c r="AL67" s="174"/>
     </row>
     <row r="68" spans="1:38" s="51" customFormat="1">
       <c r="A68" s="103" t="s">
@@ -5152,8 +5245,8 @@
       <c r="S68" s="15"/>
       <c r="T68" s="15"/>
       <c r="Y68" s="15"/>
-      <c r="AK68" s="159"/>
-      <c r="AL68" s="159"/>
+      <c r="AK68" s="174"/>
+      <c r="AL68" s="174"/>
     </row>
     <row r="69" spans="1:38" s="51" customFormat="1">
       <c r="A69" s="104" t="s">
@@ -5191,7 +5284,7 @@
       <c r="S69" s="15"/>
       <c r="T69" s="15"/>
       <c r="Y69" s="15"/>
-      <c r="AK69" s="159"/>
+      <c r="AK69" s="174"/>
       <c r="AL69" s="140"/>
     </row>
     <row r="70" spans="1:38" s="51" customFormat="1">
@@ -5230,8 +5323,8 @@
       <c r="S70" s="15"/>
       <c r="T70" s="15"/>
       <c r="Y70" s="15"/>
-      <c r="AK70" s="159"/>
-      <c r="AL70" s="159"/>
+      <c r="AK70" s="174"/>
+      <c r="AL70" s="174"/>
     </row>
     <row r="71" spans="1:38" s="51" customFormat="1">
       <c r="A71" s="105" t="s">
@@ -5269,8 +5362,8 @@
       <c r="S71" s="15"/>
       <c r="T71" s="15"/>
       <c r="Y71" s="15"/>
-      <c r="AK71" s="159"/>
-      <c r="AL71" s="159"/>
+      <c r="AK71" s="174"/>
+      <c r="AL71" s="174"/>
     </row>
     <row r="72" spans="1:38" s="51" customFormat="1">
       <c r="A72" s="105" t="s">
@@ -5308,8 +5401,8 @@
       <c r="S72" s="15"/>
       <c r="T72" s="15"/>
       <c r="Y72" s="15"/>
-      <c r="AK72" s="159"/>
-      <c r="AL72" s="159"/>
+      <c r="AK72" s="174"/>
+      <c r="AL72" s="174"/>
     </row>
     <row r="73" spans="1:38" s="51" customFormat="1">
       <c r="A73" s="105" t="s">
@@ -5347,8 +5440,8 @@
       <c r="S73" s="15"/>
       <c r="T73" s="15"/>
       <c r="Y73" s="15"/>
-      <c r="AK73" s="159"/>
-      <c r="AL73" s="159"/>
+      <c r="AK73" s="174"/>
+      <c r="AL73" s="174"/>
     </row>
     <row r="74" spans="1:38" s="51" customFormat="1">
       <c r="A74" s="103" t="s">
@@ -5386,8 +5479,8 @@
       <c r="S74" s="15"/>
       <c r="T74" s="15"/>
       <c r="Y74" s="15"/>
-      <c r="AK74" s="159"/>
-      <c r="AL74" s="159"/>
+      <c r="AK74" s="174"/>
+      <c r="AL74" s="174"/>
     </row>
     <row r="75" spans="1:38" s="51" customFormat="1" ht="15.5" customHeight="1">
       <c r="A75" s="102" t="s">
@@ -5425,8 +5518,8 @@
       <c r="S75" s="15"/>
       <c r="T75" s="15"/>
       <c r="Y75" s="15"/>
-      <c r="AK75" s="159"/>
-      <c r="AL75" s="159"/>
+      <c r="AK75" s="174"/>
+      <c r="AL75" s="174"/>
     </row>
     <row r="76" spans="1:38" s="51" customFormat="1">
       <c r="A76" s="105" t="s">
@@ -5464,8 +5557,8 @@
       <c r="S76" s="15"/>
       <c r="T76" s="15"/>
       <c r="Y76" s="15"/>
-      <c r="AK76" s="159"/>
-      <c r="AL76" s="159"/>
+      <c r="AK76" s="174"/>
+      <c r="AL76" s="174"/>
     </row>
     <row r="77" spans="1:38" s="51" customFormat="1">
       <c r="A77" s="105" t="s">
@@ -5503,8 +5596,8 @@
       <c r="S77" s="15"/>
       <c r="T77" s="15"/>
       <c r="Y77" s="15"/>
-      <c r="AK77" s="159"/>
-      <c r="AL77" s="159"/>
+      <c r="AK77" s="174"/>
+      <c r="AL77" s="174"/>
     </row>
     <row r="78" spans="1:38" s="51" customFormat="1">
       <c r="A78" s="105" t="s">
@@ -5542,8 +5635,8 @@
       <c r="S78" s="15"/>
       <c r="T78" s="15"/>
       <c r="Y78" s="15"/>
-      <c r="AK78" s="159"/>
-      <c r="AL78" s="159"/>
+      <c r="AK78" s="174"/>
+      <c r="AL78" s="174"/>
     </row>
     <row r="79" spans="1:38" s="51" customFormat="1">
       <c r="A79" s="105" t="s">
@@ -5581,8 +5674,8 @@
       <c r="S79" s="15"/>
       <c r="T79" s="15"/>
       <c r="Y79" s="15"/>
-      <c r="AK79" s="159"/>
-      <c r="AL79" s="159"/>
+      <c r="AK79" s="174"/>
+      <c r="AL79" s="174"/>
     </row>
     <row r="80" spans="1:38" s="51" customFormat="1">
       <c r="A80" s="103" t="s">
@@ -5620,8 +5713,8 @@
       <c r="S80" s="15"/>
       <c r="T80" s="15"/>
       <c r="Y80" s="15"/>
-      <c r="AK80" s="159"/>
-      <c r="AL80" s="159"/>
+      <c r="AK80" s="174"/>
+      <c r="AL80" s="174"/>
     </row>
     <row r="81" spans="1:38" s="51" customFormat="1">
       <c r="A81" s="104" t="s">
@@ -5698,8 +5791,8 @@
       <c r="S82" s="15"/>
       <c r="T82" s="15"/>
       <c r="Y82" s="15"/>
-      <c r="AK82" s="159"/>
-      <c r="AL82" s="159"/>
+      <c r="AK82" s="174"/>
+      <c r="AL82" s="174"/>
     </row>
     <row r="83" spans="1:38" s="51" customFormat="1">
       <c r="A83" s="105" t="s">
@@ -5737,8 +5830,8 @@
       <c r="S83" s="15"/>
       <c r="T83" s="15"/>
       <c r="Y83" s="15"/>
-      <c r="AK83" s="159"/>
-      <c r="AL83" s="159"/>
+      <c r="AK83" s="174"/>
+      <c r="AL83" s="174"/>
     </row>
     <row r="84" spans="1:38" s="51" customFormat="1">
       <c r="A84" s="103" t="s">
@@ -5776,8 +5869,8 @@
       <c r="S84" s="15"/>
       <c r="T84" s="15"/>
       <c r="Y84" s="15"/>
-      <c r="AK84" s="159"/>
-      <c r="AL84" s="159"/>
+      <c r="AK84" s="174"/>
+      <c r="AL84" s="174"/>
     </row>
     <row r="85" spans="1:38" s="51" customFormat="1">
       <c r="A85" s="102" t="s">
@@ -5816,8 +5909,8 @@
       <c r="T85" s="15"/>
       <c r="Y85" s="90"/>
       <c r="Z85" s="90"/>
-      <c r="AK85" s="159"/>
-      <c r="AL85" s="159"/>
+      <c r="AK85" s="174"/>
+      <c r="AL85" s="174"/>
     </row>
     <row r="86" spans="1:38" s="51" customFormat="1">
       <c r="A86" s="105" t="s">
@@ -5856,8 +5949,8 @@
       <c r="T86" s="15"/>
       <c r="Y86" s="90"/>
       <c r="Z86" s="90"/>
-      <c r="AK86" s="159"/>
-      <c r="AL86" s="159"/>
+      <c r="AK86" s="174"/>
+      <c r="AL86" s="174"/>
     </row>
     <row r="87" spans="1:38" s="51" customFormat="1">
       <c r="A87" s="105" t="s">
@@ -5896,8 +5989,8 @@
       <c r="T87" s="15"/>
       <c r="Y87" s="90"/>
       <c r="Z87" s="90"/>
-      <c r="AK87" s="159"/>
-      <c r="AL87" s="159"/>
+      <c r="AK87" s="174"/>
+      <c r="AL87" s="174"/>
     </row>
     <row r="88" spans="1:38" s="51" customFormat="1">
       <c r="A88" s="105" t="s">
@@ -5936,8 +6029,8 @@
       <c r="T88" s="15"/>
       <c r="Y88" s="90"/>
       <c r="Z88" s="90"/>
-      <c r="AK88" s="159"/>
-      <c r="AL88" s="159"/>
+      <c r="AK88" s="174"/>
+      <c r="AL88" s="174"/>
     </row>
     <row r="89" spans="1:38" s="51" customFormat="1">
       <c r="A89" s="105" t="s">
@@ -5975,8 +6068,8 @@
       <c r="S89" s="15"/>
       <c r="T89" s="15"/>
       <c r="Y89" s="90"/>
-      <c r="AK89" s="159"/>
-      <c r="AL89" s="159"/>
+      <c r="AK89" s="174"/>
+      <c r="AL89" s="174"/>
     </row>
     <row r="90" spans="1:38" s="51" customFormat="1">
       <c r="A90" s="103" t="s">
@@ -6014,8 +6107,8 @@
       <c r="S90" s="15"/>
       <c r="T90" s="15"/>
       <c r="Y90" s="90"/>
-      <c r="AK90" s="159"/>
-      <c r="AL90" s="159"/>
+      <c r="AK90" s="174"/>
+      <c r="AL90" s="174"/>
     </row>
     <row r="91" spans="1:38" s="51" customFormat="1">
       <c r="A91" s="102" t="s">
@@ -6053,8 +6146,8 @@
       <c r="S91" s="15"/>
       <c r="T91" s="15"/>
       <c r="Y91" s="15"/>
-      <c r="AK91" s="159"/>
-      <c r="AL91" s="159"/>
+      <c r="AK91" s="174"/>
+      <c r="AL91" s="174"/>
     </row>
     <row r="92" spans="1:38" s="51" customFormat="1">
       <c r="A92" s="105" t="s">
@@ -6092,8 +6185,8 @@
       <c r="S92" s="15"/>
       <c r="T92" s="15"/>
       <c r="Y92" s="15"/>
-      <c r="AK92" s="159"/>
-      <c r="AL92" s="159"/>
+      <c r="AK92" s="174"/>
+      <c r="AL92" s="174"/>
     </row>
     <row r="93" spans="1:38" s="51" customFormat="1">
       <c r="A93" s="103" t="s">
@@ -6131,8 +6224,8 @@
       <c r="S93" s="15"/>
       <c r="T93" s="15"/>
       <c r="Y93" s="15"/>
-      <c r="AK93" s="159"/>
-      <c r="AL93" s="159"/>
+      <c r="AK93" s="174"/>
+      <c r="AL93" s="174"/>
     </row>
     <row r="94" spans="1:38" s="51" customFormat="1">
       <c r="A94" s="102" t="s">
@@ -6170,8 +6263,8 @@
       <c r="S94" s="15"/>
       <c r="T94" s="15"/>
       <c r="Y94" s="15"/>
-      <c r="AK94" s="159"/>
-      <c r="AL94" s="159"/>
+      <c r="AK94" s="174"/>
+      <c r="AL94" s="174"/>
     </row>
     <row r="95" spans="1:38" s="51" customFormat="1">
       <c r="A95" s="105" t="s">
@@ -6209,8 +6302,8 @@
       <c r="S95" s="15"/>
       <c r="T95" s="15"/>
       <c r="Y95" s="15"/>
-      <c r="AK95" s="159"/>
-      <c r="AL95" s="159"/>
+      <c r="AK95" s="174"/>
+      <c r="AL95" s="174"/>
     </row>
     <row r="96" spans="1:38" s="51" customFormat="1">
       <c r="A96" s="103" t="s">
@@ -6248,8 +6341,8 @@
       <c r="S96" s="15"/>
       <c r="T96" s="15"/>
       <c r="Y96" s="15"/>
-      <c r="AK96" s="159"/>
-      <c r="AL96" s="159"/>
+      <c r="AK96" s="174"/>
+      <c r="AL96" s="174"/>
     </row>
     <row r="97" spans="1:41" s="51" customFormat="1" ht="15.5" customHeight="1">
       <c r="A97" s="102" t="s">
@@ -6287,8 +6380,8 @@
       <c r="S97" s="15"/>
       <c r="T97" s="15"/>
       <c r="Y97" s="15"/>
-      <c r="AK97" s="159"/>
-      <c r="AL97" s="159"/>
+      <c r="AK97" s="174"/>
+      <c r="AL97" s="174"/>
     </row>
     <row r="98" spans="1:41" s="51" customFormat="1">
       <c r="A98" s="105" t="s">
@@ -6326,8 +6419,8 @@
       <c r="S98" s="15"/>
       <c r="T98" s="15"/>
       <c r="Y98" s="15"/>
-      <c r="AK98" s="159"/>
-      <c r="AL98" s="159"/>
+      <c r="AK98" s="174"/>
+      <c r="AL98" s="174"/>
     </row>
     <row r="99" spans="1:41" s="51" customFormat="1">
       <c r="A99" s="105" t="s">
@@ -6365,8 +6458,8 @@
       <c r="S99" s="15"/>
       <c r="T99" s="15"/>
       <c r="Y99" s="15"/>
-      <c r="AK99" s="159"/>
-      <c r="AL99" s="159"/>
+      <c r="AK99" s="174"/>
+      <c r="AL99" s="174"/>
     </row>
     <row r="100" spans="1:41" s="51" customFormat="1">
       <c r="A100" s="105" t="s">
@@ -6404,8 +6497,8 @@
       <c r="S100" s="15"/>
       <c r="T100" s="15"/>
       <c r="Y100" s="15"/>
-      <c r="AK100" s="159"/>
-      <c r="AL100" s="159"/>
+      <c r="AK100" s="174"/>
+      <c r="AL100" s="174"/>
     </row>
     <row r="101" spans="1:41" s="51" customFormat="1">
       <c r="A101" s="105" t="s">
@@ -6443,8 +6536,8 @@
       <c r="S101" s="15"/>
       <c r="T101" s="15"/>
       <c r="Y101" s="15"/>
-      <c r="AK101" s="159"/>
-      <c r="AL101" s="159"/>
+      <c r="AK101" s="174"/>
+      <c r="AL101" s="174"/>
     </row>
     <row r="102" spans="1:41" s="51" customFormat="1">
       <c r="A102" s="103" t="s">
@@ -6482,8 +6575,8 @@
       <c r="S102" s="15"/>
       <c r="T102" s="15"/>
       <c r="Y102" s="15"/>
-      <c r="AK102" s="159"/>
-      <c r="AL102" s="159"/>
+      <c r="AK102" s="174"/>
+      <c r="AL102" s="174"/>
     </row>
     <row r="103" spans="1:41" s="51" customFormat="1">
       <c r="A103" s="102" t="s">
@@ -6521,8 +6614,8 @@
       <c r="S103" s="15"/>
       <c r="T103" s="15"/>
       <c r="Y103" s="15"/>
-      <c r="AK103" s="159"/>
-      <c r="AL103" s="159"/>
+      <c r="AK103" s="174"/>
+      <c r="AL103" s="174"/>
     </row>
     <row r="104" spans="1:41" s="51" customFormat="1">
       <c r="A104" s="103" t="s">
@@ -6560,8 +6653,8 @@
       <c r="S104" s="15"/>
       <c r="T104" s="15"/>
       <c r="Y104" s="15"/>
-      <c r="AK104" s="159"/>
-      <c r="AL104" s="159"/>
+      <c r="AK104" s="174"/>
+      <c r="AL104" s="174"/>
     </row>
     <row r="105" spans="1:41" s="51" customFormat="1" ht="15.5" customHeight="1">
       <c r="A105" s="102" t="s">
@@ -6599,8 +6692,8 @@
       <c r="S105" s="15"/>
       <c r="T105" s="15"/>
       <c r="Y105" s="15"/>
-      <c r="AK105" s="159"/>
-      <c r="AL105" s="159"/>
+      <c r="AK105" s="174"/>
+      <c r="AL105" s="174"/>
     </row>
     <row r="106" spans="1:41" s="51" customFormat="1">
       <c r="A106" s="103" t="s">
@@ -6638,8 +6731,8 @@
       <c r="S106" s="15"/>
       <c r="T106" s="15"/>
       <c r="Y106" s="15"/>
-      <c r="AK106" s="159"/>
-      <c r="AL106" s="159"/>
+      <c r="AK106" s="174"/>
+      <c r="AL106" s="174"/>
     </row>
     <row r="107" spans="1:41" s="51" customFormat="1" ht="15.5" customHeight="1">
       <c r="A107" s="102" t="s">
@@ -6677,8 +6770,8 @@
       <c r="S107" s="15"/>
       <c r="T107" s="15"/>
       <c r="Y107" s="15"/>
-      <c r="AK107" s="159"/>
-      <c r="AL107" s="159"/>
+      <c r="AK107" s="174"/>
+      <c r="AL107" s="174"/>
     </row>
     <row r="108" spans="1:41" s="51" customFormat="1">
       <c r="A108" s="105" t="s">
@@ -6716,8 +6809,8 @@
       <c r="S108" s="15"/>
       <c r="T108" s="15"/>
       <c r="Y108" s="15"/>
-      <c r="AK108" s="159"/>
-      <c r="AL108" s="159"/>
+      <c r="AK108" s="174"/>
+      <c r="AL108" s="174"/>
     </row>
     <row r="109" spans="1:41" s="74" customFormat="1">
       <c r="A109" s="103" t="s">
@@ -6766,8 +6859,8 @@
       <c r="AH109" s="51"/>
       <c r="AI109" s="51"/>
       <c r="AJ109" s="51"/>
-      <c r="AK109" s="159"/>
-      <c r="AL109" s="159"/>
+      <c r="AK109" s="174"/>
+      <c r="AL109" s="174"/>
       <c r="AM109" s="51"/>
       <c r="AN109" s="51"/>
       <c r="AO109" s="51"/>
@@ -18139,6 +18232,632 @@
       <c r="AN459" s="41"/>
       <c r="AO459" s="41"/>
     </row>
+    <row r="462" spans="1:41" s="162" customFormat="1">
+      <c r="A462" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="B462" s="158" t="s">
+        <v>400</v>
+      </c>
+      <c r="C462" s="159"/>
+      <c r="D462" s="158"/>
+      <c r="E462" s="158"/>
+      <c r="F462" s="158"/>
+      <c r="G462" s="160"/>
+      <c r="H462" s="160"/>
+      <c r="I462" s="160"/>
+      <c r="J462" s="160"/>
+      <c r="K462" s="161"/>
+      <c r="L462" s="160"/>
+      <c r="M462" s="160"/>
+      <c r="N462" s="160"/>
+      <c r="O462" s="160"/>
+      <c r="P462" s="160"/>
+      <c r="Q462" s="160"/>
+      <c r="R462" s="160"/>
+      <c r="S462" s="160"/>
+      <c r="T462" s="160"/>
+      <c r="Y462" s="163"/>
+      <c r="Z462" s="163"/>
+      <c r="AA462" s="163"/>
+      <c r="AB462" s="163"/>
+      <c r="AC462" s="163"/>
+      <c r="AD462" s="163"/>
+      <c r="AE462" s="163"/>
+      <c r="AF462" s="163"/>
+      <c r="AG462" s="163"/>
+      <c r="AH462" s="163"/>
+      <c r="AI462" s="163"/>
+      <c r="AJ462" s="163"/>
+      <c r="AK462" s="163"/>
+      <c r="AL462" s="163"/>
+      <c r="AM462" s="163"/>
+      <c r="AN462" s="163"/>
+      <c r="AO462" s="163"/>
+    </row>
+    <row r="463" spans="1:41" s="163" customFormat="1">
+      <c r="A463" s="164" t="s">
+        <v>20</v>
+      </c>
+      <c r="B463" s="165">
+        <v>1</v>
+      </c>
+      <c r="C463" s="166"/>
+      <c r="D463" s="164"/>
+      <c r="E463" s="164"/>
+      <c r="F463" s="164"/>
+      <c r="G463" s="164"/>
+      <c r="H463" s="164"/>
+      <c r="I463" s="164"/>
+      <c r="J463" s="164"/>
+      <c r="K463" s="164"/>
+      <c r="L463" s="164"/>
+      <c r="M463" s="164"/>
+      <c r="N463" s="164"/>
+      <c r="O463" s="164"/>
+      <c r="P463" s="164"/>
+      <c r="Q463" s="164"/>
+      <c r="R463" s="164"/>
+      <c r="S463" s="164"/>
+      <c r="T463" s="164"/>
+    </row>
+    <row r="464" spans="1:41" s="163" customFormat="1">
+      <c r="A464" s="164" t="s">
+        <v>21</v>
+      </c>
+      <c r="B464" s="164" t="s">
+        <v>420</v>
+      </c>
+      <c r="C464" s="166"/>
+      <c r="D464" s="164"/>
+      <c r="E464" s="164"/>
+      <c r="F464" s="164"/>
+      <c r="G464" s="164"/>
+      <c r="H464" s="164"/>
+      <c r="I464" s="164"/>
+      <c r="J464" s="164"/>
+      <c r="K464" s="164"/>
+      <c r="L464" s="164"/>
+      <c r="M464" s="164"/>
+      <c r="N464" s="164"/>
+      <c r="O464" s="164"/>
+      <c r="P464" s="164"/>
+      <c r="Q464" s="164"/>
+      <c r="R464" s="164"/>
+      <c r="S464" s="164"/>
+      <c r="T464" s="164"/>
+    </row>
+    <row r="465" spans="1:20" s="163" customFormat="1">
+      <c r="A465" s="164" t="s">
+        <v>22</v>
+      </c>
+      <c r="B465" s="165">
+        <v>1</v>
+      </c>
+      <c r="C465" s="166"/>
+      <c r="D465" s="164"/>
+      <c r="E465" s="164"/>
+      <c r="F465" s="164"/>
+      <c r="G465" s="164"/>
+      <c r="H465" s="164"/>
+      <c r="I465" s="164"/>
+      <c r="J465" s="164"/>
+      <c r="K465" s="164"/>
+      <c r="L465" s="164"/>
+      <c r="M465" s="164"/>
+      <c r="N465" s="164"/>
+      <c r="O465" s="164"/>
+      <c r="P465" s="164"/>
+      <c r="Q465" s="164"/>
+      <c r="R465" s="164"/>
+      <c r="S465" s="164"/>
+      <c r="T465" s="164"/>
+    </row>
+    <row r="466" spans="1:20" s="163" customFormat="1">
+      <c r="A466" s="164" t="s">
+        <v>23</v>
+      </c>
+      <c r="B466" s="164" t="s">
+        <v>419</v>
+      </c>
+      <c r="C466" s="166"/>
+      <c r="D466" s="164"/>
+      <c r="E466" s="164"/>
+      <c r="F466" s="164"/>
+      <c r="G466" s="164"/>
+      <c r="H466" s="164"/>
+      <c r="I466" s="164"/>
+      <c r="J466" s="164"/>
+      <c r="K466" s="164"/>
+      <c r="L466" s="164"/>
+      <c r="M466" s="164"/>
+      <c r="N466" s="164"/>
+      <c r="O466" s="164"/>
+      <c r="P466" s="164"/>
+      <c r="Q466" s="164"/>
+      <c r="R466" s="164"/>
+      <c r="S466" s="164"/>
+      <c r="T466" s="164"/>
+    </row>
+    <row r="467" spans="1:20" s="163" customFormat="1">
+      <c r="A467" s="164" t="s">
+        <v>24</v>
+      </c>
+      <c r="B467" s="164" t="s">
+        <v>401</v>
+      </c>
+      <c r="C467" s="166"/>
+      <c r="D467" s="164"/>
+      <c r="E467" s="164"/>
+      <c r="F467" s="164"/>
+      <c r="G467" s="164"/>
+      <c r="H467" s="164"/>
+      <c r="I467" s="164"/>
+      <c r="J467" s="164"/>
+      <c r="K467" s="164"/>
+      <c r="L467" s="164"/>
+      <c r="M467" s="164"/>
+      <c r="N467" s="164"/>
+      <c r="O467" s="164"/>
+      <c r="P467" s="164"/>
+      <c r="Q467" s="164"/>
+      <c r="R467" s="164"/>
+      <c r="S467" s="164"/>
+      <c r="T467" s="164"/>
+    </row>
+    <row r="468" spans="1:20" s="163" customFormat="1">
+      <c r="A468" s="164" t="s">
+        <v>26</v>
+      </c>
+      <c r="B468" s="164" t="s">
+        <v>54</v>
+      </c>
+      <c r="C468" s="166"/>
+      <c r="D468" s="164"/>
+      <c r="E468" s="164"/>
+      <c r="F468" s="164"/>
+      <c r="G468" s="164"/>
+      <c r="H468" s="167"/>
+      <c r="I468" s="167"/>
+      <c r="J468" s="164"/>
+      <c r="K468" s="164"/>
+      <c r="L468" s="164"/>
+      <c r="M468" s="164"/>
+      <c r="N468" s="164"/>
+      <c r="O468" s="164"/>
+      <c r="P468" s="164"/>
+      <c r="Q468" s="164"/>
+      <c r="R468" s="164"/>
+      <c r="S468" s="164"/>
+      <c r="T468" s="164"/>
+    </row>
+    <row r="469" spans="1:20" s="163" customFormat="1">
+      <c r="A469" s="167" t="s">
+        <v>27</v>
+      </c>
+      <c r="B469" s="167"/>
+      <c r="C469" s="168"/>
+      <c r="D469" s="167"/>
+      <c r="E469" s="167"/>
+      <c r="F469" s="167"/>
+      <c r="G469" s="167"/>
+      <c r="H469" s="164"/>
+      <c r="I469" s="164"/>
+      <c r="J469" s="164"/>
+      <c r="K469" s="164"/>
+      <c r="L469" s="164"/>
+      <c r="M469" s="164"/>
+      <c r="N469" s="164"/>
+      <c r="O469" s="164"/>
+      <c r="P469" s="164"/>
+      <c r="Q469" s="164"/>
+      <c r="R469" s="164"/>
+      <c r="S469" s="164"/>
+      <c r="T469" s="164"/>
+    </row>
+    <row r="470" spans="1:20" s="163" customFormat="1">
+      <c r="A470" s="167" t="s">
+        <v>28</v>
+      </c>
+      <c r="B470" s="167" t="s">
+        <v>29</v>
+      </c>
+      <c r="C470" s="168" t="s">
+        <v>24</v>
+      </c>
+      <c r="D470" s="167" t="s">
+        <v>26</v>
+      </c>
+      <c r="E470" s="167" t="s">
+        <v>30</v>
+      </c>
+      <c r="F470" s="167" t="s">
+        <v>31</v>
+      </c>
+      <c r="G470" s="167" t="s">
+        <v>23</v>
+      </c>
+      <c r="H470" s="167" t="s">
+        <v>21</v>
+      </c>
+      <c r="I470" s="167" t="s">
+        <v>32</v>
+      </c>
+      <c r="J470" s="169" t="s">
+        <v>33</v>
+      </c>
+      <c r="K470" s="169" t="s">
+        <v>34</v>
+      </c>
+      <c r="L470" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="M470" s="169" t="s">
+        <v>36</v>
+      </c>
+      <c r="N470" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="O470" s="169" t="s">
+        <v>38</v>
+      </c>
+      <c r="P470" s="169" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q470" s="169" t="s">
+        <v>40</v>
+      </c>
+      <c r="R470" s="169" t="s">
+        <v>41</v>
+      </c>
+      <c r="S470" s="167" t="s">
+        <v>42</v>
+      </c>
+      <c r="T470" s="169" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="471" spans="1:20" s="163" customFormat="1">
+      <c r="A471" s="164" t="str">
+        <f>B462</f>
+        <v>ammonia production, steam reforming, liquid</v>
+      </c>
+      <c r="B471" s="165">
+        <v>1</v>
+      </c>
+      <c r="C471" s="166" t="str">
+        <f>B467</f>
+        <v>FR</v>
+      </c>
+      <c r="D471" s="164" t="str">
+        <f>B468</f>
+        <v>kilogram</v>
+      </c>
+      <c r="E471" s="164"/>
+      <c r="F471" s="164" t="s">
+        <v>44</v>
+      </c>
+      <c r="G471" s="164"/>
+      <c r="H471" s="164"/>
+      <c r="I471" s="164"/>
+      <c r="J471" s="170"/>
+      <c r="K471" s="170"/>
+      <c r="L471" s="170"/>
+      <c r="M471" s="170"/>
+      <c r="N471" s="170"/>
+      <c r="O471" s="170"/>
+      <c r="P471" s="170"/>
+      <c r="Q471" s="170"/>
+      <c r="R471" s="170"/>
+      <c r="S471" s="164"/>
+      <c r="T471" s="170"/>
+    </row>
+    <row r="472" spans="1:20" s="163" customFormat="1">
+      <c r="A472" s="164" t="s">
+        <v>402</v>
+      </c>
+      <c r="B472" s="165">
+        <v>3.9047009913655199E-10</v>
+      </c>
+      <c r="C472" s="164" t="s">
+        <v>53</v>
+      </c>
+      <c r="D472" s="164" t="s">
+        <v>26</v>
+      </c>
+      <c r="E472" s="164"/>
+      <c r="F472" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G472" s="164" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="473" spans="1:20" s="163" customFormat="1">
+      <c r="A473" s="164" t="s">
+        <v>403</v>
+      </c>
+      <c r="B473" s="165">
+        <v>-1.9523504956827601E-4</v>
+      </c>
+      <c r="C473" s="164" t="s">
+        <v>25</v>
+      </c>
+      <c r="D473" s="164" t="s">
+        <v>54</v>
+      </c>
+      <c r="E473" s="164"/>
+      <c r="F473" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G473" s="164" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="474" spans="1:20" s="163" customFormat="1">
+      <c r="A474" s="164" t="s">
+        <v>226</v>
+      </c>
+      <c r="B474" s="165">
+        <v>3.4166133674448299E-4</v>
+      </c>
+      <c r="C474" s="164" t="s">
+        <v>53</v>
+      </c>
+      <c r="D474" s="164" t="s">
+        <v>54</v>
+      </c>
+      <c r="E474" s="164"/>
+      <c r="F474" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G474" s="164" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="475" spans="1:20" s="163" customFormat="1">
+      <c r="A475" s="164" t="s">
+        <v>404</v>
+      </c>
+      <c r="B475" s="165">
+        <v>2.92852574352414E-5</v>
+      </c>
+      <c r="C475" s="164" t="s">
+        <v>53</v>
+      </c>
+      <c r="D475" s="164" t="s">
+        <v>54</v>
+      </c>
+      <c r="E475" s="164"/>
+      <c r="F475" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G475" s="164" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="476" spans="1:20" s="163" customFormat="1">
+      <c r="A476" s="164" t="s">
+        <v>405</v>
+      </c>
+      <c r="B476" s="165">
+        <v>0.70382235369363599</v>
+      </c>
+      <c r="C476" s="164" t="s">
+        <v>162</v>
+      </c>
+      <c r="D476" s="164" t="s">
+        <v>54</v>
+      </c>
+      <c r="E476" s="164"/>
+      <c r="F476" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G476" s="164" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="477" spans="1:20" s="163" customFormat="1">
+      <c r="A477" s="164" t="s">
+        <v>406</v>
+      </c>
+      <c r="B477" s="165">
+        <v>0.22777422449632101</v>
+      </c>
+      <c r="C477" s="164" t="s">
+        <v>401</v>
+      </c>
+      <c r="D477" s="164" t="s">
+        <v>81</v>
+      </c>
+      <c r="E477" s="164"/>
+      <c r="F477" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G477" s="164" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="478" spans="1:20" s="163" customFormat="1">
+      <c r="A478" s="164" t="s">
+        <v>407</v>
+      </c>
+      <c r="B478" s="165">
+        <v>0.60576910557780295</v>
+      </c>
+      <c r="C478" s="164" t="s">
+        <v>401</v>
+      </c>
+      <c r="D478" s="164" t="s">
+        <v>129</v>
+      </c>
+      <c r="E478" s="164"/>
+      <c r="F478" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G478" s="164" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="479" spans="1:20" s="163" customFormat="1">
+      <c r="A479" s="164" t="s">
+        <v>407</v>
+      </c>
+      <c r="B479" s="165">
+        <v>4.3404243230599797E-3</v>
+      </c>
+      <c r="C479" s="164" t="s">
+        <v>401</v>
+      </c>
+      <c r="D479" s="164" t="s">
+        <v>129</v>
+      </c>
+      <c r="E479" s="164"/>
+      <c r="F479" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G479" s="164" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="480" spans="1:20" s="163" customFormat="1">
+      <c r="A480" s="164" t="s">
+        <v>406</v>
+      </c>
+      <c r="B480" s="165">
+        <v>5.543607647</v>
+      </c>
+      <c r="C480" s="164" t="s">
+        <v>401</v>
+      </c>
+      <c r="D480" s="164" t="s">
+        <v>81</v>
+      </c>
+      <c r="E480" s="164"/>
+      <c r="F480" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G480" s="164" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="481" spans="1:7" s="163" customFormat="1">
+      <c r="A481" s="164" t="s">
+        <v>138</v>
+      </c>
+      <c r="B481" s="165">
+        <v>1.40569235689158</v>
+      </c>
+      <c r="C481" s="164"/>
+      <c r="D481" s="164" t="s">
+        <v>54</v>
+      </c>
+      <c r="E481" s="164" t="s">
+        <v>413</v>
+      </c>
+      <c r="F481" s="164" t="s">
+        <v>85</v>
+      </c>
+      <c r="G481" s="164"/>
+    </row>
+    <row r="482" spans="1:7" s="163" customFormat="1">
+      <c r="A482" s="164" t="s">
+        <v>154</v>
+      </c>
+      <c r="B482" s="165">
+        <v>6.8332267348896695E-4</v>
+      </c>
+      <c r="C482" s="164"/>
+      <c r="D482" s="164" t="s">
+        <v>54</v>
+      </c>
+      <c r="E482" s="164" t="s">
+        <v>413</v>
+      </c>
+      <c r="F482" s="164" t="s">
+        <v>85</v>
+      </c>
+      <c r="G482" s="164"/>
+    </row>
+    <row r="483" spans="1:7" s="163" customFormat="1">
+      <c r="A483" s="164" t="s">
+        <v>416</v>
+      </c>
+      <c r="B483" s="165">
+        <v>5.31039334825711E-2</v>
+      </c>
+      <c r="C483" s="164"/>
+      <c r="D483" s="164" t="s">
+        <v>129</v>
+      </c>
+      <c r="E483" s="164" t="s">
+        <v>134</v>
+      </c>
+      <c r="F483" s="164" t="s">
+        <v>85</v>
+      </c>
+      <c r="G483" s="164"/>
+    </row>
+    <row r="484" spans="1:7" s="163" customFormat="1">
+      <c r="A484" s="164" t="s">
+        <v>417</v>
+      </c>
+      <c r="B484" s="165">
+        <v>1.17141029740965E-4</v>
+      </c>
+      <c r="C484" s="164"/>
+      <c r="D484" s="164" t="s">
+        <v>54</v>
+      </c>
+      <c r="E484" s="164" t="s">
+        <v>414</v>
+      </c>
+      <c r="F484" s="164" t="s">
+        <v>85</v>
+      </c>
+      <c r="G484" s="164"/>
+    </row>
+    <row r="485" spans="1:7" s="163" customFormat="1">
+      <c r="A485" s="164" t="s">
+        <v>416</v>
+      </c>
+      <c r="B485" s="165">
+        <v>8.4405480892228907E-2</v>
+      </c>
+      <c r="C485" s="164"/>
+      <c r="D485" s="164" t="s">
+        <v>129</v>
+      </c>
+      <c r="E485" s="164" t="s">
+        <v>414</v>
+      </c>
+      <c r="F485" s="164" t="s">
+        <v>85</v>
+      </c>
+      <c r="G485" s="164"/>
+    </row>
+    <row r="486" spans="1:7" s="172" customFormat="1">
+      <c r="A486" s="171" t="s">
+        <v>418</v>
+      </c>
+      <c r="B486" s="175">
+        <v>0.13666453469779299</v>
+      </c>
+      <c r="C486" s="171"/>
+      <c r="D486" s="171" t="s">
+        <v>129</v>
+      </c>
+      <c r="E486" s="171" t="s">
+        <v>415</v>
+      </c>
+      <c r="F486" s="171" t="s">
+        <v>85</v>
+      </c>
+      <c r="G486" s="171"/>
+    </row>
+    <row r="489" spans="1:7">
+      <c r="B489" s="176"/>
+    </row>
   </sheetData>
   <mergeCells count="27">
     <mergeCell ref="AK82:AK84"/>
@@ -18175,6 +18894,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4f559a66-d13b-41c5-989e-96cb258a4f2a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="61f6d602-005f-4e3e-90ae-fc5077fd546f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F1800535943334EB4E0E883E610E294" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b3882544b11b37512790aea260cd5d53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4f559a66-d13b-41c5-989e-96cb258a4f2a" xmlns:ns3="61f6d602-005f-4e3e-90ae-fc5077fd546f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="039aa0795ac0dca1182382d4fd2aa2c5" ns2:_="" ns3:_="">
     <xsd:import namespace="4f559a66-d13b-41c5-989e-96cb258a4f2a"/>
@@ -18385,7 +19115,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -18394,18 +19124,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4f559a66-d13b-41c5-989e-96cb258a4f2a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="61f6d602-005f-4e3e-90ae-fc5077fd546f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C69714-70F1-46A8-9F8E-A48D1CFFCA24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4f559a66-d13b-41c5-989e-96cb258a4f2a"/>
+    <ds:schemaRef ds:uri="61f6d602-005f-4e3e-90ae-fc5077fd546f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E1E1FF1-99FB-4D84-92D6-551478C71E32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18424,21 +19154,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35807B10-B905-4B9D-8A85-35426E94F7D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C69714-70F1-46A8-9F8E-A48D1CFFCA24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4f559a66-d13b-41c5-989e-96cb258a4f2a"/>
-    <ds:schemaRef ds:uri="61f6d602-005f-4e3e-90ae-fc5077fd546f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
daily restriction added to pv
</commit_message>
<xml_diff>
--- a/electrolyzers_LCI.xlsx
+++ b/electrolyzers_LCI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsteinbach\PycharmProjects\HySPI app\HySPI_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6623E8D0-AE06-4ACF-B8AB-F9E414BED6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AE574C-FFF9-42CA-917E-4D127AD3F0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1EA9BED0-42EC-4F80-9B46-2A73048EBAB6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2314" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="424">
   <si>
     <t>skip</t>
   </si>
@@ -1327,6 +1327,15 @@
   </si>
   <si>
     <t>adapted from ecoinvent data</t>
+  </si>
+  <si>
+    <t>ammonia production, hydrogen, liquid</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>some activity</t>
   </si>
 </sst>
 </file>
@@ -2647,10 +2656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E518564-62B5-463A-BC83-0EAFF50C141D}">
-  <dimension ref="A1:AO513"/>
+  <dimension ref="A1:AO514"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A470" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B474" sqref="B474"/>
+    <sheetView tabSelected="1" topLeftCell="A487" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B500" sqref="B500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
@@ -18859,7 +18868,7 @@
         <v>19</v>
       </c>
       <c r="B489" s="158" t="s">
-        <v>400</v>
+        <v>421</v>
       </c>
       <c r="C489" s="159"/>
       <c r="D489" s="158"/>
@@ -19142,7 +19151,7 @@
     <row r="498" spans="1:20" s="163" customFormat="1">
       <c r="A498" s="164" t="str">
         <f>B489</f>
-        <v>ammonia production, steam reforming, liquid</v>
+        <v>ammonia production, hydrogen, liquid</v>
       </c>
       <c r="B498" s="165">
         <v>1</v>
@@ -19284,7 +19293,7 @@
         <v>406</v>
       </c>
       <c r="B504" s="165">
-        <v>0.22777422449632101</v>
+        <v>0.64</v>
       </c>
       <c r="C504" s="164" t="s">
         <v>401</v>
@@ -19302,80 +19311,79 @@
     </row>
     <row r="505" spans="1:20" s="163" customFormat="1">
       <c r="A505" s="164" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B505" s="165">
-        <v>0.60576910557780295</v>
+        <f>0.823 * 0.37</f>
+        <v>0.30451</v>
       </c>
       <c r="C505" s="164" t="s">
         <v>401</v>
       </c>
       <c r="D505" s="164" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="E505" s="164"/>
       <c r="F505" s="164" t="s">
         <v>46</v>
       </c>
       <c r="G505" s="164" t="s">
-        <v>412</v>
+        <v>82</v>
       </c>
     </row>
     <row r="506" spans="1:20" s="163" customFormat="1">
       <c r="A506" s="164" t="s">
-        <v>407</v>
+        <v>422</v>
       </c>
       <c r="B506" s="165">
-        <v>4.3404243230599797E-3</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="C506" s="164" t="s">
         <v>401</v>
       </c>
       <c r="D506" s="164" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
       <c r="E506" s="164"/>
       <c r="F506" s="164" t="s">
         <v>46</v>
       </c>
       <c r="G506" s="164" t="s">
-        <v>412</v>
+        <v>82</v>
       </c>
     </row>
     <row r="507" spans="1:20" s="163" customFormat="1">
       <c r="A507" s="164" t="s">
-        <v>406</v>
+        <v>154</v>
       </c>
       <c r="B507" s="165">
-        <v>5.543607647</v>
-      </c>
-      <c r="C507" s="164" t="s">
-        <v>401</v>
-      </c>
+        <v>6.8332267348896695E-4</v>
+      </c>
+      <c r="C507" s="164"/>
       <c r="D507" s="164" t="s">
-        <v>81</v>
-      </c>
-      <c r="E507" s="164"/>
+        <v>54</v>
+      </c>
+      <c r="E507" s="164" t="s">
+        <v>413</v>
+      </c>
       <c r="F507" s="164" t="s">
-        <v>46</v>
-      </c>
-      <c r="G507" s="164" t="s">
-        <v>82</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="G507" s="164"/>
     </row>
     <row r="508" spans="1:20" s="163" customFormat="1">
       <c r="A508" s="164" t="s">
-        <v>138</v>
+        <v>416</v>
       </c>
       <c r="B508" s="165">
-        <v>1.40569235689158</v>
+        <v>5.31039334825711E-2</v>
       </c>
       <c r="C508" s="164"/>
       <c r="D508" s="164" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="E508" s="164" t="s">
-        <v>413</v>
+        <v>134</v>
       </c>
       <c r="F508" s="164" t="s">
         <v>85</v>
@@ -19384,17 +19392,17 @@
     </row>
     <row r="509" spans="1:20" s="163" customFormat="1">
       <c r="A509" s="164" t="s">
-        <v>154</v>
+        <v>417</v>
       </c>
       <c r="B509" s="165">
-        <v>6.8332267348896695E-4</v>
+        <v>1.17141029740965E-4</v>
       </c>
       <c r="C509" s="164"/>
       <c r="D509" s="164" t="s">
         <v>54</v>
       </c>
       <c r="E509" s="164" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F509" s="164" t="s">
         <v>85</v>
@@ -19406,76 +19414,46 @@
         <v>416</v>
       </c>
       <c r="B510" s="165">
-        <v>5.31039334825711E-2</v>
+        <v>8.4405480892228907E-2</v>
       </c>
       <c r="C510" s="164"/>
       <c r="D510" s="164" t="s">
         <v>129</v>
       </c>
       <c r="E510" s="164" t="s">
-        <v>134</v>
+        <v>414</v>
       </c>
       <c r="F510" s="164" t="s">
         <v>85</v>
       </c>
       <c r="G510" s="164"/>
     </row>
-    <row r="511" spans="1:20" s="163" customFormat="1">
-      <c r="A511" s="164" t="s">
-        <v>417</v>
-      </c>
-      <c r="B511" s="165">
-        <v>1.17141029740965E-4</v>
-      </c>
-      <c r="C511" s="164"/>
-      <c r="D511" s="164" t="s">
-        <v>54</v>
-      </c>
-      <c r="E511" s="164" t="s">
-        <v>414</v>
-      </c>
-      <c r="F511" s="164" t="s">
+    <row r="511" spans="1:20" s="172" customFormat="1">
+      <c r="A511" s="171" t="s">
+        <v>418</v>
+      </c>
+      <c r="B511" s="173">
+        <v>0.13666453469779299</v>
+      </c>
+      <c r="C511" s="171"/>
+      <c r="D511" s="171" t="s">
+        <v>129</v>
+      </c>
+      <c r="E511" s="171" t="s">
+        <v>415</v>
+      </c>
+      <c r="F511" s="171" t="s">
         <v>85</v>
       </c>
-      <c r="G511" s="164"/>
-    </row>
-    <row r="512" spans="1:20" s="163" customFormat="1">
-      <c r="A512" s="164" t="s">
-        <v>416</v>
-      </c>
-      <c r="B512" s="165">
-        <v>8.4405480892228907E-2</v>
-      </c>
-      <c r="C512" s="164"/>
-      <c r="D512" s="164" t="s">
-        <v>129</v>
-      </c>
-      <c r="E512" s="164" t="s">
-        <v>414</v>
-      </c>
-      <c r="F512" s="164" t="s">
-        <v>85</v>
-      </c>
-      <c r="G512" s="164"/>
-    </row>
-    <row r="513" spans="1:7" s="172" customFormat="1">
-      <c r="A513" s="171" t="s">
-        <v>418</v>
-      </c>
-      <c r="B513" s="173">
-        <v>0.13666453469779299</v>
-      </c>
-      <c r="C513" s="171"/>
-      <c r="D513" s="171" t="s">
-        <v>129</v>
-      </c>
-      <c r="E513" s="171" t="s">
-        <v>415</v>
-      </c>
-      <c r="F513" s="171" t="s">
-        <v>85</v>
-      </c>
-      <c r="G513" s="171"/>
+      <c r="G511" s="171"/>
+    </row>
+    <row r="514" spans="1:2">
+      <c r="A514" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="B514" s="158" t="s">
+        <v>423</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="27">

</xml_diff>